<commit_message>
add line in presence2
</commit_message>
<xml_diff>
--- a/workOnExcel/presence2.xlsx
+++ b/workOnExcel/presence2.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\project\Group2_Yesodot\workOnExcel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD395E-0F07-4A5E-85E1-585A1846304B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="presence" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>index</t>
   </si>
@@ -140,17 +134,26 @@
   </si>
   <si>
     <t>Wed, 19 Dec 2018 11:12:42</t>
+  </si>
+  <si>
+    <t>michi</t>
+  </si>
+  <si>
+    <t>tsho</t>
+  </si>
+  <si>
+    <t>Wed, 19 Dec 2018 12:04:26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -183,19 +186,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -237,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,27 +264,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -321,24 +298,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,21 +473,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -583,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -609,7 +561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -638,7 +590,7 @@
         <v>37373</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -667,7 +619,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -696,7 +648,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -725,7 +677,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -752,6 +704,29 @@
       </c>
       <c r="I8">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worker and s. manager can get presence report
</commit_message>
<xml_diff>
--- a/workOnExcel/presence2.xlsx
+++ b/workOnExcel/presence2.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\project\Group2_Yesodot\workOnExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8522FC21-AA63-4A30-8D10-B9CC385863AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="presence" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>index</t>
   </si>
@@ -100,30 +106,15 @@
     <t>zorin</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 21:42:40</t>
-  </si>
-  <si>
     <t>Sun, 16 Dec 2018 21:44:32</t>
   </si>
   <si>
-    <t>jeck</t>
-  </si>
-  <si>
-    <t>ka</t>
-  </si>
-  <si>
     <t>Wed, 19 Dec 2018 10:49:50</t>
   </si>
   <si>
     <t>Wed, 19 Dec 2018 10:54:41</t>
   </si>
   <si>
-    <t>joni</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
     <t>Wed, 19 Dec 2018 11:12:36</t>
   </si>
   <si>
@@ -146,17 +137,20 @@
   </si>
   <si>
     <t>Wed, 19 Dec 2018 12:09:07</t>
+  </si>
+  <si>
+    <t>Sun, 17 Dec 2018 21:42:40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -189,11 +183,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,9 +269,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,6 +321,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,14 +514,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -537,8 +581,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -563,8 +610,11 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -593,7 +643,7 @@
         <v>37373</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -622,7 +672,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -633,36 +683,36 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -674,65 +724,65 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
         <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
       </c>
       <c r="I9">
         <v>281</v>

</xml_diff>

<commit_message>
manager can get presence report
</commit_message>
<xml_diff>
--- a/workOnExcel/presence2.xlsx
+++ b/workOnExcel/presence2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\project\Group2_Yesodot\workOnExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8522FC21-AA63-4A30-8D10-B9CC385863AB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6683F939-41E3-47EF-84D3-E4C272535A0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>index</t>
   </si>
@@ -55,9 +55,6 @@
     <t>hadad</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 18:08:16</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>sss</t>
   </si>
   <si>
-    <t>Sun, 16 Dec 2018 21:08:16</t>
-  </si>
-  <si>
     <t>Sun, 16 Dec 2018 21:27:02</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>Wed, 19 Dec 2018 10:54:41</t>
   </si>
   <si>
-    <t>Wed, 19 Dec 2018 11:12:36</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
@@ -140,6 +131,15 @@
   </si>
   <si>
     <t>Sun, 17 Dec 2018 21:42:40</t>
+  </si>
+  <si>
+    <t>Sun, 16 Nov 2018 18:08:16</t>
+  </si>
+  <si>
+    <t>Sun, 16 Oct 2018 21:08:16</t>
+  </si>
+  <si>
+    <t>Wed, 19 Oct 2018 11:12:36</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -567,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
       <c r="F2">
         <v>16</v>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>373</v>
@@ -590,16 +590,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="E3">
+        <v>11</v>
       </c>
       <c r="F3">
         <v>16</v>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>112</v>
@@ -619,16 +619,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>16</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4">
         <v>37373</v>
@@ -648,16 +648,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
       </c>
       <c r="F5">
         <v>16</v>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5">
         <v>1126</v>
@@ -677,16 +677,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>17</v>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>112</v>
@@ -706,16 +706,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>19</v>
@@ -724,7 +724,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7">
         <v>291</v>
@@ -735,25 +735,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -764,25 +764,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
       </c>
       <c r="I9">
         <v>281</v>

</xml_diff>